<commit_message>
rename GameScript to ScriptComponent
</commit_message>
<xml_diff>
--- a/Documents/Task_Requirements.xlsx
+++ b/Documents/Task_Requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <r>
       <t>主菜单和本地化</t>
@@ -36,9 +36,6 @@
     </r>
   </si>
   <si>
-    <t>控制坦克导航，瞄准目标，射击</t>
-  </si>
-  <si>
     <t>基于组件化的设计</t>
   </si>
   <si>
@@ -491,18 +488,12 @@
     <t>zsc</t>
   </si>
   <si>
-    <t>实现了摄像机的位移和转动</t>
-  </si>
-  <si>
     <t>目前执行详情</t>
   </si>
   <si>
     <t>计划执行</t>
   </si>
   <si>
-    <t>有了文本显示功能后，测试获取位置与转角是否正确</t>
-  </si>
-  <si>
     <t>3D音效</t>
   </si>
   <si>
@@ -524,12 +515,6 @@
     <t>cyl</t>
   </si>
   <si>
-    <t>imgui</t>
-  </si>
-  <si>
-    <t>实现菜单与游戏对象属性界面</t>
-  </si>
-  <si>
     <t>zzy</t>
   </si>
   <si>
@@ -549,6 +534,33 @@
   </si>
   <si>
     <t>zzy,zsc</t>
+  </si>
+  <si>
+    <t>完成引擎部分的摄像机</t>
+  </si>
+  <si>
+    <t>实现游戏部分的摄像机类，将其封装成摄像机组件</t>
+  </si>
+  <si>
+    <t>基本几何体的gameobject创建与component的创建</t>
+  </si>
+  <si>
+    <t>根据需求实现创造组件的接口</t>
+  </si>
+  <si>
+    <t>可以播放2d音效</t>
+  </si>
+  <si>
+    <t>3d音效的实现？</t>
+  </si>
+  <si>
+    <t>gameobejct，transform，rendercomponent</t>
+  </si>
+  <si>
+    <t>gamescript与摄像机组件的</t>
+  </si>
+  <si>
+    <t>控制坦克,导航，瞄准目标，射击</t>
   </si>
 </sst>
 </file>
@@ -575,7 +587,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,12 +603,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,7 +629,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,7 +913,7 @@
   <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -916,207 +922,217 @@
     <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
+      <c r="D4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="4" customFormat="1">
+      <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>71</v>
+      <c r="B11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
-        <v>68</v>
-      </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1124,21 +1140,21 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
         <v>55</v>
       </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
         <v>58</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1146,7 +1162,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1169,12 +1185,12 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1184,62 +1200,62 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:1">
@@ -1247,27 +1263,27 @@
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -1275,47 +1291,47 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:1">
@@ -1323,17 +1339,17 @@
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:1">
@@ -1341,27 +1357,27 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add normal to vertex
</commit_message>
<xml_diff>
--- a/Documents/Task_Requirements.xlsx
+++ b/Documents/Task_Requirements.xlsx
@@ -21,142 +21,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
   <si>
-    <r>
-      <t>主菜单和本地化</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                              </t>
-    </r>
-  </si>
-  <si>
     <t>基于组件化的设计</t>
   </si>
   <si>
     <t>坦克的炮台必须有动画</t>
   </si>
   <si>
-    <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ai</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>敌人，能够移动，攻击角色，导航绕过障碍</t>
-    </r>
-  </si>
-  <si>
     <t>存在障碍，可以处理坦克和障碍之间的碰撞</t>
   </si>
   <si>
-    <r>
-      <t>声音：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bgm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>和</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>se</t>
-    </r>
-  </si>
-  <si>
     <t>输入：按键映射</t>
   </si>
   <si>
     <t>粒子系统：火焰和炸弹的粒子</t>
   </si>
   <si>
-    <r>
-      <t>射击的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cutscene</t>
-    </r>
-  </si>
-  <si>
     <t>给导弹添加物理</t>
   </si>
   <si>
     <t>能够编辑地图的编辑器</t>
-  </si>
-  <si>
-    <r>
-      <t>打印</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fps</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>到屏幕</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">本地化      </t>
@@ -223,55 +106,7 @@
     <t>撰写技术设计文档</t>
   </si>
   <si>
-    <r>
-      <t>使用</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dx11</t>
-    </r>
-  </si>
-  <si>
     <t>不使用游戏引擎</t>
-  </si>
-  <si>
-    <r>
-      <t>支持</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>windows</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>和</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ps4</t>
-    </r>
   </si>
   <si>
     <r>
@@ -290,38 +125,12 @@
     <t>了解基本的游戏理念：</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">TPS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>，</t>
-    </r>
-  </si>
-  <si>
     <t>游戏主循环，渲染</t>
   </si>
   <si>
     <t>基于组件的编程</t>
   </si>
   <si>
-    <r>
-      <t>ai</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>，寻路</t>
-    </r>
-  </si>
-  <si>
     <t>菜单，本地化，加载，关卡</t>
   </si>
   <si>
@@ -335,21 +144,6 @@
   </si>
   <si>
     <t>dx</t>
-  </si>
-  <si>
-    <r>
-      <t>熟悉</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>git</t>
-    </r>
   </si>
   <si>
     <t>项目检测</t>
@@ -417,29 +211,6 @@
     <t>实现基本的物理碰撞检测</t>
   </si>
   <si>
-    <r>
-      <t>使用</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>gitlab</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="DengXian"/>
-      </rPr>
-      <t>进行版本控制</t>
-    </r>
-  </si>
-  <si>
     <t>ai</t>
   </si>
   <si>
@@ -561,13 +332,46 @@
   </si>
   <si>
     <t>ai寻路及避开障碍</t>
+  </si>
+  <si>
+    <t xml:space="preserve">主菜单和本地化                              </t>
+  </si>
+  <si>
+    <t>1个ai敌人，能够移动，攻击角色，导航绕过障碍</t>
+  </si>
+  <si>
+    <t>声音：bgm和se</t>
+  </si>
+  <si>
+    <t>射击的cutscene</t>
+  </si>
+  <si>
+    <t>打印fps到屏幕</t>
+  </si>
+  <si>
+    <t>使用gitlab进行版本控制</t>
+  </si>
+  <si>
+    <t>使用dx11</t>
+  </si>
+  <si>
+    <t>支持windows和ps4</t>
+  </si>
+  <si>
+    <t>TPS ，</t>
+  </si>
+  <si>
+    <t>ai，寻路</t>
+  </si>
+  <si>
+    <t>熟悉git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,8 +390,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,6 +431,21 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -616,10 +456,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -630,8 +473,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -928,211 +783,211 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1">
       <c r="A11" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1140,24 +995,24 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1165,7 +1020,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1188,105 +1043,105 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:1">
+      <c r="A35" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="2" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:1">
+      <c r="A40" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="1" t="s">
+    <row r="41" spans="1:1">
+      <c r="A41" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="1" t="s">
+    <row r="43" spans="1:1">
+      <c r="A43" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="1" t="s">
-        <v>11</v>
+      <c r="A44" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="2"/>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="1" t="s">
-        <v>29</v>
+      <c r="A46" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="1" t="s">
-        <v>54</v>
+      <c r="A47" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="1" t="s">
-        <v>30</v>
+      <c r="A48" s="7" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="1" t="s">
-        <v>31</v>
+      <c r="A49" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="1" t="s">
-        <v>32</v>
+      <c r="A50" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -1294,65 +1149,65 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="2" t="s">
-        <v>35</v>
+      <c r="A54" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="1" t="s">
-        <v>36</v>
+      <c r="A55" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="1" t="s">
-        <v>37</v>
+      <c r="A56" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="2" t="s">
-        <v>38</v>
+      <c r="A57" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="1" t="s">
-        <v>39</v>
+      <c r="A58" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="1" t="s">
-        <v>40</v>
+      <c r="A59" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="1" t="s">
-        <v>41</v>
+      <c r="A60" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="2"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="1" t="s">
-        <v>42</v>
+      <c r="A62" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="2" t="s">
-        <v>43</v>
+      <c r="A63" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="1" t="s">
-        <v>44</v>
+      <c r="A64" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:1">
@@ -1360,27 +1215,27 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
realize PlayerTank and PlayerController gameplay logic
</commit_message>
<xml_diff>
--- a/Documents/Task_Requirements.xlsx
+++ b/Documents/Task_Requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
   <si>
     <t>基于组件化的设计</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>菜单，本地化，加载，关卡</t>
-  </si>
-  <si>
-    <t>效果，碰撞，物理，声音，输入，材质，纹理</t>
   </si>
   <si>
     <t>游戏配置文件</t>
@@ -365,6 +362,45 @@
   </si>
   <si>
     <t>熟悉git</t>
+  </si>
+  <si>
+    <t>菜单</t>
+  </si>
+  <si>
+    <t>关卡</t>
+  </si>
+  <si>
+    <t>本地化</t>
+  </si>
+  <si>
+    <t>加载</t>
+  </si>
+  <si>
+    <t>特效，碰撞，物理，声音，输入，材质，纹理</t>
+  </si>
+  <si>
+    <t>特效</t>
+  </si>
+  <si>
+    <t>碰撞物理</t>
+  </si>
+  <si>
+    <t>声音</t>
+  </si>
+  <si>
+    <t>输入</t>
+  </si>
+  <si>
+    <t>材质</t>
+  </si>
+  <si>
+    <t>纹理</t>
+  </si>
+  <si>
+    <t>本周完成</t>
+  </si>
+  <si>
+    <t>本周完成控制，瞄准</t>
   </si>
 </sst>
 </file>
@@ -462,7 +498,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -482,6 +518,9 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -765,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -792,13 +831,13 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -825,7 +864,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -852,142 +891,142 @@
         <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="E15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -995,24 +1034,24 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1020,7 +1059,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1053,161 +1092,197 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:2">
       <c r="A35" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:2">
       <c r="A38" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:2">
       <c r="A40" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:2">
       <c r="A41" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:2">
       <c r="A43" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:2">
       <c r="A44" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:2">
       <c r="A46" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:2">
       <c r="A47" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:7">
       <c r="A49" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:7">
       <c r="A54" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:7">
       <c r="A56" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:7">
       <c r="A57" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="6" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="2"/>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="7" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:7">
       <c r="A64" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:1">
@@ -1215,27 +1290,27 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add AnimationTitle and complete opening animation
</commit_message>
<xml_diff>
--- a/Documents/Task_Requirements.xlsx
+++ b/Documents/Task_Requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
   <si>
     <t>基于组件化的设计</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>本周完成控制，瞄准</t>
+  </si>
+  <si>
+    <t>制作其他的cutscene</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -519,7 +522,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
@@ -807,7 +809,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1091,12 +1093,12 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B33" t="s">
@@ -1145,9 +1147,12 @@
       <c r="A41" s="6" t="s">
         <v>87</v>
       </c>
+      <c r="B41" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1218,7 +1223,7 @@
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="7" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1229,13 +1234,13 @@
       <c r="B58" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D58" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E58" s="10" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1243,7 +1248,7 @@
       <c r="A59" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C59" s="9" t="s">
@@ -1263,7 +1268,7 @@
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="7" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>